<commit_message>
Updated formatting and fixed some comments
</commit_message>
<xml_diff>
--- a/Back-end Recommender & Converter/GameData.xlsx
+++ b/Back-end Recommender & Converter/GameData.xlsx
@@ -14,45 +14,87 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>D/Generation HD</t>
   </si>
   <si>
-    <t>Title: D/Generation HD
-Description: The year is 2021  and Genoq has become a leading corporation in bio-medical research. However the tower  some 90 stories high  is not all that it seems. Somewhere within the tower  highly illegal bio-weapons research has been conducted in secret. June 26th  disaster strikes and the lethal organic weapons have escaped and threaten not only the staff members stranded in the tower  but the world itself. You arrive on the 80th floor with an urgent package addressed to Derrida  the lead scientist at Genoq working on the bio-weapons research. Set back from your goal  you must climb the tower  assisting those in need or focusing solely on your task at hand  and stopping the virus from escaping the tower and threatening all life on the planet.Will you help the stranded survivors or hinder them  Can you deliver the package to Derrida in time  Can you prevent the impending catastrophe and escape with your life Key Features New high res graphics New music by Mark   x27 TDK  x27  Knight New control menu Can save at any point in the game Leaderboards Achievements Same great gameplay
-Genres: Adventure, Puzzle
-Tags: Full controller support, Steam Achievements, Steam Leaderboards, Retro, Singleplayer
-Developers: West Coast Software, West Coast Software Limited
-Publishers: West Coast Software, West Coast Software Limited
-Platforms: PC, macOS, Xbox One, PlayStation 4, Nintendo Switch
-Places To Purchase: https://www.nintendo.com/games/detail/d-generation-hd-switch, http://store.steampowered.com/app/389740/, https://store.playstation.com/en-us/product/UP1640-CUSA04221_00-0000000000000001, https://www.microsoft.com/en-us/store/p/d-generation-hd/c2tnxshx530h</t>
+    <t>Title: D/Generation HD</t>
+  </si>
+  <si>
+    <t>Description: The year is 2021  and Genoq has become a leading corporation in bio-medical research. However the tower  some 90 stories high  is not all that it seems. Somewhere within the tower  highly illegal bio-weapons research has been conducted in secret. June 26th  disaster strikes and the lethal organic weapons have escaped and threaten not only the staff members stranded in the tower  but the world itself. You arrive on the 80th floor with an urgent package addressed to Derrida  the lead scientist at Genoq working on the bio-weapons research. Set back from your goal  you must climb the tower  assisting those in need or focusing solely on your task at hand  and stopping the virus from escaping the tower and threatening all life on the planet.Will you help the stranded survivors or hinder them  Can you deliver the package to Derrida in time  Can you prevent the impending catastrophe and escape with your life Key Features New high res graphics New music by Mark   x27 TDK  x27  Knight New control menu Can save at any point in the game Leaderboards Achievements Same great gameplay</t>
+  </si>
+  <si>
+    <t>Genres: Adventure, Puzzle</t>
+  </si>
+  <si>
+    <t>Tags: Full controller support, Steam Achievements, Steam Leaderboards, Retro, Singleplayer</t>
+  </si>
+  <si>
+    <t>Developers: West Coast Software, West Coast Software Limited</t>
+  </si>
+  <si>
+    <t>Publishers: West Coast Software, West Coast Software Limited</t>
+  </si>
+  <si>
+    <t>Platforms: PC, macOS, Xbox One, PlayStation 4, Nintendo Switch</t>
+  </si>
+  <si>
+    <t>Places To Purchase: https://www.nintendo.com/games/detail/d-generation-hd-switch, http://store.steampowered.com/app/389740/, https://store.playstation.com/en-us/product/UP1640-CUSA04221_00-0000000000000001, https://www.microsoft.com/en-us/store/p/d-generation-hd/c2tnxshx530h</t>
   </si>
   <si>
     <t>Extreme Exorcism</t>
   </si>
   <si>
-    <t>Title: Extreme Exorcism
-Description: Extreme Exorcism is a paranormal platformer where every move you make comes back to haunt you.Take on the role of Mae Barrons  an Extreme Exorcist with extreme measures. Her supernatural skills are called upon when everything and everyone else has failed to rid a haunted house of its ghostly presence.Conventional methods wont cut it with these ghosts. Instead  Mae comes armed with a deadly arsenal of ghost-busting weapons  from rocket launchers to razor sharp boomerangs.But these arent your average poltergeists. At the end of each round  a ghost appears and mimics your every move from the round before. The longer you survive the more extreme the game becomes.Engage in non-stop ghost annihilation in 10 eerie areas of the haunted house  each room presenting its own hellish hazard. Brave the winds on the balcony and the fire in the kitchen  surviving for as long as you can. With a devilish local multiplayer  you can play co-op or deathmatch modes with up to 3 of your friends  and with 50 unique challenges even the most daring Extreme Exorcist will be put to the test.
-Genres: Action, Adventure, Casual, Indie
-Tags: 2D, Full controller support, Steam Achievements, Steam Leaderboards, Co-op, Horror, Multiplayer, Pixel Graphics, Singleplayer, Split Screen, cooperative, steam-trading-cards, stats
-Developers: Golden Ruby Games
-Publishers: Ripstone, Ripstone Ltd
-Platforms: macOS, PC, Xbox One, Wii U, PlayStation 3, PlayStation 4
-Places To Purchase: https://store.playstation.com/en-us/product/UP2070-NPUB31699_00-EXTREMEXORCISM01, https://www.microsoft.com/en-us/p/extreme-exorcism/c00k010531v9?cid=msft_web_chart, https://www.nintendo.com/games/detail/mjkhibi71vhmzwqby2yyflg1kjoroz2_, http://store.steampowered.com/app/334100/</t>
+    <t>Title: Extreme Exorcism</t>
+  </si>
+  <si>
+    <t>Description: Extreme Exorcism is a paranormal platformer where every move you make comes back to haunt you.Take on the role of Mae Barrons  an Extreme Exorcist with extreme measures. Her supernatural skills are called upon when everything and everyone else has failed to rid a haunted house of its ghostly presence.Conventional methods wont cut it with these ghosts. Instead  Mae comes armed with a deadly arsenal of ghost-busting weapons  from rocket launchers to razor sharp boomerangs.But these arent your average poltergeists. At the end of each round  a ghost appears and mimics your every move from the round before. The longer you survive the more extreme the game becomes.Engage in non-stop ghost annihilation in 10 eerie areas of the haunted house  each room presenting its own hellish hazard. Brave the winds on the balcony and the fire in the kitchen  surviving for as long as you can. With a devilish local multiplayer  you can play co-op or deathmatch modes with up to 3 of your friends  and with 50 unique challenges even the most daring Extreme Exorcist will be put to the test.</t>
+  </si>
+  <si>
+    <t>Genres: Action, Adventure, Casual, Indie</t>
+  </si>
+  <si>
+    <t>Tags: 2D, Full controller support, Steam Achievements, Steam Leaderboards, Co-op, Horror, Multiplayer, Pixel Graphics, Singleplayer, Split Screen, cooperative, steam-trading-cards, stats</t>
+  </si>
+  <si>
+    <t>Developers: Golden Ruby Games</t>
+  </si>
+  <si>
+    <t>Publishers: Ripstone, Ripstone Ltd</t>
+  </si>
+  <si>
+    <t>Platforms: macOS, PC, Xbox One, Wii U, PlayStation 3, PlayStation 4</t>
+  </si>
+  <si>
+    <t>Places To Purchase: https://store.playstation.com/en-us/product/UP2070-NPUB31699_00-EXTREMEXORCISM01, https://www.microsoft.com/en-us/p/extreme-exorcism/c00k010531v9?cid=msft_web_chart, https://www.nintendo.com/games/detail/mjkhibi71vhmzwqby2yyflg1kjoroz2_, http://store.steampowered.com/app/334100/</t>
   </si>
   <si>
     <t>Toto Temple Deluxe</t>
   </si>
   <si>
-    <t>Title: Toto Temple Deluxe
-Description:  quot Toto Temple Deluxe is near perfect and delivers an amazing party experience quot - Rares Gruian  8WorldsNews  quot It  x27 s simple and addictive - what a multiplayer game should be. quot - Mysterious Indiecade Judge quot It  x27 s fun  it  x27 s crazy  and you  x27 ll undoubtedly be yelling. quot - Alpha  N4G  quot It is stupidly fun. You  x27 ll likely find yourself standing in front of the screen  yelling at your fellow goat stealers and jostling them in real life. quot - Dan Tynan  Yahoo Toto Temple Deluxe is a fast-paced  local-multiplayer king-of-the-hill style game in which players must steal an egg-laying goat from their friends and try to keep it on their own head for as long as possible. You know  normal stuff.Dashing GameplayInfinitely dash in any direction to swiftly move around and powerfully headbutt the goat carrier to steal its four-legged booty. Escape your jealous opponents and protect the goat by blocking their attacks with a well-timed shield pop  Youll  quot get their goat quot   guaranteed.Classic ModeProve youre the ultimate shepherd in Classic mode: Gather 3k points first by holding on to the goat  collecting coins hatched from goat eggs  yeah dont ask  and harnessing the power of powerful power-ups  Play as teams or in free-for-all.Bomb ModeBlast everyones face off in Bomb mode: Be the first to grab the explosive goat  we know  stop interrupting us  and keep it long enough for it to detonate near your soon-to-be-dead rivals. Lose the goat and the timer resets  Play as teams or in free-for-all.TemplesEach temple offers a unique  exploitable mechanic for you to discover. Use them wisely and outsmart your opponents like they dont even... what  how did you.. BotsBots will play with you whenever you want and for as long as you want. They never complain. They also never open up your fridge and ask if they can eat that pizza slice you got left from last night. Bots are awesome. Oh  and you can change their difficulty level too  because they will probably kick your ass-tonishing little bottom.
-Genres: Action, Casual, Indie
-Tags: Full controller support, 4 Player Local, Steam Achievements, Steam Cloud, Steam Leaderboards, Co-op, Local Co-Op, Local Multiplayer, Multiplayer, Singleplayer, Split Screen, party, stats
-Developers: Juicy Beast, Juicy Beast Studio, JUICY BEAST STUDIO LTD.
-Publishers: Juicy Beast, Juicy Beast Studio
-Platforms: PC, Xbox One, Wii U, PlayStation 4
-Places To Purchase: https://www.nintendo.com/games/detail/toto-temple-deluxe-wii-u, http://store.steampowered.com/app/342920/, https://store.playstation.com/en-us/product/UP0384-CUSA01775_00-TOTOTEMPLEDELUXE, https://www.microsoft.com/en-us/store/p/toto-temple-deluxe/c4q4m8f9xkg6</t>
+    <t>Title: Toto Temple Deluxe</t>
+  </si>
+  <si>
+    <t>Description:  quot Toto Temple Deluxe is near perfect and delivers an amazing party experience quot - Rares Gruian  8WorldsNews  quot It  x27 s simple and addictive - what a multiplayer game should be. quot - Mysterious Indiecade Judge quot It  x27 s fun  it  x27 s crazy  and you  x27 ll undoubtedly be yelling. quot - Alpha  N4G  quot It is stupidly fun. You  x27 ll likely find yourself standing in front of the screen  yelling at your fellow goat stealers and jostling them in real life. quot - Dan Tynan  Yahoo Toto Temple Deluxe is a fast-paced  local-multiplayer king-of-the-hill style game in which players must steal an egg-laying goat from their friends and try to keep it on their own head for as long as possible. You know  normal stuff.Dashing GameplayInfinitely dash in any direction to swiftly move around and powerfully headbutt the goat carrier to steal its four-legged booty. Escape your jealous opponents and protect the goat by blocking their attacks with a well-timed shield pop  Youll  quot get their goat quot   guaranteed.Classic ModeProve youre the ultimate shepherd in Classic mode: Gather 3k points first by holding on to the goat  collecting coins hatched from goat eggs  yeah dont ask  and harnessing the power of powerful power-ups  Play as teams or in free-for-all.Bomb ModeBlast everyones face off in Bomb mode: Be the first to grab the explosive goat  we know  stop interrupting us  and keep it long enough for it to detonate near your soon-to-be-dead rivals. Lose the goat and the timer resets  Play as teams or in free-for-all.TemplesEach temple offers a unique  exploitable mechanic for you to discover. Use them wisely and outsmart your opponents like they dont even... what  how did you.. BotsBots will play with you whenever you want and for as long as you want. They never complain. They also never open up your fridge and ask if they can eat that pizza slice you got left from last night. Bots are awesome. Oh  and you can change their difficulty level too  because they will probably kick your ass-tonishing little bottom.</t>
+  </si>
+  <si>
+    <t>Genres: Action, Casual, Indie</t>
+  </si>
+  <si>
+    <t>Tags: Full controller support, 4 Player Local, Steam Achievements, Steam Cloud, Steam Leaderboards, Co-op, Local Co-Op, Local Multiplayer, Multiplayer, Singleplayer, Split Screen, party, stats</t>
+  </si>
+  <si>
+    <t>Developers: Juicy Beast, Juicy Beast Studio, JUICY BEAST STUDIO LTD.</t>
+  </si>
+  <si>
+    <t>Publishers: Juicy Beast, Juicy Beast Studio</t>
+  </si>
+  <si>
+    <t>Platforms: PC, Xbox One, Wii U, PlayStation 4</t>
+  </si>
+  <si>
+    <t>Places To Purchase: https://www.nintendo.com/games/detail/toto-temple-deluxe-wii-u, http://store.steampowered.com/app/342920/, https://store.playstation.com/en-us/product/UP0384-CUSA01775_00-TOTOTEMPLEDELUXE, https://www.microsoft.com/en-us/store/p/toto-temple-deluxe/c4q4m8f9xkg6</t>
   </si>
 </sst>
 </file>
@@ -384,34 +426,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merged Data Extraction and Recommendation
Done to prevent discrepancies between the data and for easier access in the database.
</commit_message>
<xml_diff>
--- a/Back-end Recommender & Converter/GameData.xlsx
+++ b/Back-end Recommender & Converter/GameData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>D/Generation HD</t>
   </si>
@@ -43,6 +43,21 @@
     <t>Places To Purchase: https://www.nintendo.com/games/detail/d-generation-hd-switch, http://store.steampowered.com/app/389740/, https://store.playstation.com/en-us/product/UP1640-CUSA04221_00-0000000000000001, https://www.microsoft.com/en-us/store/p/d-generation-hd/c2tnxshx530h</t>
   </si>
   <si>
+    <t>Super Strawberry Man</t>
+  </si>
+  <si>
+    <t>Death Fungeon</t>
+  </si>
+  <si>
+    <t>Hello Neighbor</t>
+  </si>
+  <si>
+    <t>AR-K</t>
+  </si>
+  <si>
+    <t>Spaceship Looter</t>
+  </si>
+  <si>
     <t>Extreme Exorcism</t>
   </si>
   <si>
@@ -70,6 +85,21 @@
     <t>Places To Purchase: https://store.playstation.com/en-us/product/UP2070-NPUB31699_00-EXTREMEXORCISM01, https://www.microsoft.com/en-us/p/extreme-exorcism/c00k010531v9?cid=msft_web_chart, https://www.nintendo.com/games/detail/mjkhibi71vhmzwqby2yyflg1kjoroz2_, http://store.steampowered.com/app/334100/</t>
   </si>
   <si>
+    <t>Imprisoned Light</t>
+  </si>
+  <si>
+    <t>Over 9000 Zombies!</t>
+  </si>
+  <si>
+    <t>Tic-Toc-Tower</t>
+  </si>
+  <si>
+    <t>TowerFall Ascension</t>
+  </si>
+  <si>
+    <t>Straima</t>
+  </si>
+  <si>
     <t>Toto Temple Deluxe</t>
   </si>
   <si>
@@ -95,6 +125,21 @@
   </si>
   <si>
     <t>Places To Purchase: https://www.nintendo.com/games/detail/toto-temple-deluxe-wii-u, http://store.steampowered.com/app/342920/, https://store.playstation.com/en-us/product/UP0384-CUSA01775_00-TOTOTEMPLEDELUXE, https://www.microsoft.com/en-us/store/p/toto-temple-deluxe/c4q4m8f9xkg6</t>
+  </si>
+  <si>
+    <t>Move or Die</t>
+  </si>
+  <si>
+    <t>Dual Core</t>
+  </si>
+  <si>
+    <t>PixelJunk Nom Nom Galaxy</t>
+  </si>
+  <si>
+    <t>Streets of Red: Devil's Dare Deluxe</t>
+  </si>
+  <si>
+    <t>Nuclear Throne</t>
   </si>
 </sst>
 </file>
@@ -426,13 +471,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -460,63 +505,108 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="I2" t="s">
-        <v>17</v>
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G3" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="H3" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="I3" t="s">
-        <v>26</v>
+        <v>36</v>
+      </c>
+      <c r="J3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>